<commit_message>
Doctor list bug fixes
</commit_message>
<xml_diff>
--- a/Doctor_database.xlsx
+++ b/Doctor_database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nihal/Desktop/Virtual Assistant/Google Receptionist/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247547C7-E08C-E74C-9785-03EB5AA3BCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904E6C56-48AB-994B-99C7-FEB20FAEBFF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15480" yWindow="-900" windowWidth="15480" windowHeight="21600" xr2:uid="{ED834940-EE8E-C74D-B577-5E421CE51EB8}"/>
+    <workbookView xWindow="-22120" yWindow="-900" windowWidth="22120" windowHeight="21600" xr2:uid="{ED834940-EE8E-C74D-B577-5E421CE51EB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>Angelina Johns</t>
+  </si>
+  <si>
+    <t>Toby Mac</t>
   </si>
 </sst>
 </file>
@@ -506,7 +509,7 @@
   <dimension ref="A1:E91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A90" sqref="A90"/>
+      <selection activeCell="A87" sqref="A87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -605,7 +608,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -758,7 +761,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
@@ -911,7 +914,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B24" t="s">
         <v>30</v>
@@ -1064,7 +1067,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
@@ -1217,7 +1220,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
         <v>32</v>
@@ -1370,7 +1373,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B51" t="s">
         <v>33</v>
@@ -1487,7 +1490,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>6</v>
       </c>
@@ -1523,7 +1526,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B60" t="s">
         <v>34</v>
@@ -1676,7 +1679,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B69" t="s">
         <v>35</v>
@@ -1829,7 +1832,7 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B78" t="s">
         <v>36</v>
@@ -1982,7 +1985,7 @@
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B87" t="s">
         <v>37</v>

</xml_diff>